<commit_message>
Modified the leader_assignment function to fix few errors
</commit_message>
<xml_diff>
--- a/KAMAU FAMILY LIST.xlsx
+++ b/KAMAU FAMILY LIST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\kamau_family_contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892AAAA7-6F82-41F5-81E3-2D7029BC9A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D008D00E-2897-4E92-B9F2-BF80189817A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>HARUN WAIRUMBI</t>
   </si>
@@ -76,16 +76,10 @@
     <t>IRENE KUNGU</t>
   </si>
   <si>
-    <t>NANCY KUNGU</t>
-  </si>
-  <si>
     <t>SAM KUNGU</t>
   </si>
   <si>
     <t>JOEL KUNGU</t>
-  </si>
-  <si>
-    <t>ANN KUNGU</t>
   </si>
   <si>
     <t>VICTOR KUNGU</t>
@@ -442,20 +436,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -472,10 +466,10 @@
         <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -490,10 +484,10 @@
         <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -507,7 +501,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -521,7 +515,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -555,7 +549,7 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -563,18 +557,8 @@
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="G10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="G11" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>